<commit_message>
Company Module changes - 22 Aug 2023
</commit_message>
<xml_diff>
--- a/TestData/T2040_Companies_StandardCoverageTeam_VerifyRequiredFieldsHelpText.xlsx
+++ b/TestData/T2040_Companies_StandardCoverageTeam_VerifyRequiredFieldsHelpText.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hgandhi1012\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AB3F84-E7A2-4813-B241-6B53F603478F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -125,13 +126,13 @@
     <t>A</t>
   </si>
   <si>
-    <t>Jennifer Muller</t>
+    <t>Jacklyn Robinson</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,8 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -452,25 +452,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -480,43 +480,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
@@ -530,24 +530,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -570,7 +570,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -599,39 +599,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>

</xml_diff>